<commit_message>
New storage scenarios and degradation curves
</commit_message>
<xml_diff>
--- a/data/raw_data/degradation_curves_nsb.xlsx
+++ b/data/raw_data/degradation_curves_nsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Library/CloudStorage/Box-Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feraguilar/Library/CloudStorage/Box-Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D88B71-619A-D445-89EF-326F35E5FB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02ACA8F-23D7-7448-B6D2-46DD0021C5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{92548F31-C31D-0241-8F30-7F9E6B95A567}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{92548F31-C31D-0241-8F30-7F9E6B95A567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1134,7 +1134,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1145,11 +1145,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1419,7 +1419,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Age of battery</a:t>
+                  <a:t>Age of battery [years]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1619,37 +1619,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-NO"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3175,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9F8629-6B55-B242-BF24-8308AAED88DC}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated FIgures and storage scenarios
</commit_message>
<xml_diff>
--- a/data/raw_data/degradation_curves_nsb.xlsx
+++ b/data/raw_data/degradation_curves_nsb.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feraguilar/Library/CloudStorage/Box-Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02ACA8F-23D7-7448-B6D2-46DD0021C5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DE147E-7C8B-C347-B985-C00607733FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{92548F31-C31D-0241-8F30-7F9E6B95A567}"/>
+    <workbookView xWindow="9780" yWindow="2560" windowWidth="27320" windowHeight="14860" xr2:uid="{92548F31-C31D-0241-8F30-7F9E6B95A567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1653,6 +1654,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2809,15 +2811,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>78014</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
+      <xdr:colOff>230414</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>161472</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2842,7 +2844,709 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>762001</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>762001</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F3FF7ED-3D49-ABFA-5AC9-2F0558E46737}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10033001" y="3602182"/>
+          <a:ext cx="0" cy="4260273"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>221674</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>94673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>221674</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>184727</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA1ED85-5807-704D-9B01-9C6FDD2543EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11155219" y="5082309"/>
+          <a:ext cx="0" cy="2791691"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466437</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>96981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466437</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DDEB3D-0C1F-B440-8655-51DD0E015FB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8906164" y="4253345"/>
+          <a:ext cx="0" cy="3609110"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>496455</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>108527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>501074</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9D7B8D-C1E1-F940-88F1-01BF8CE841BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12261273" y="5511800"/>
+          <a:ext cx="4619" cy="2350655"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>168563</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>87745</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>173181</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>196272</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C823A33A-0F98-0541-8FA8-DEBE2E539812}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7777018" y="3828472"/>
+          <a:ext cx="4618" cy="4057073"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.52823</cdr:x>
+      <cdr:y>0.30981</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.67656</cdr:x>
+      <cdr:y>0.37003</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1D2946-710B-7A34-EAE3-3D55A18C3289}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5788891" y="2417618"/>
+          <a:ext cx="1625510" cy="469945"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600"/>
+            <a:t>Mean lifetime</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.54088</cdr:x>
+      <cdr:y>0.58648</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.68921</cdr:x>
+      <cdr:y>0.6467</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CC223C-B350-6613-58CC-0C2F2C52F727}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5927436" y="4576618"/>
+          <a:ext cx="1625619" cy="469946"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>68% of</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> values</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.49041</cdr:x>
+      <cdr:y>0.63737</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.69558</cdr:x>
+      <cdr:y>0.63737</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8090967F-3D5A-DCEF-D447-6F841E3AE6C6}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5374409" y="4973781"/>
+          <a:ext cx="2248395" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53456</cdr:x>
+      <cdr:y>0.70632</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.68289</cdr:x>
+      <cdr:y>0.76654</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEB10DC6-5C73-24F7-67AB-4D0E5B88B29B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5858163" y="5511801"/>
+          <a:ext cx="1625619" cy="469946"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>99% of</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> values</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.389</cdr:x>
+      <cdr:y>0.75886</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.79672</cdr:x>
+      <cdr:y>0.75886</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7022F969-B851-18C0-5D64-7A133E1C0F69}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4263077" y="5921828"/>
+          <a:ext cx="4468091" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3144,8 +3848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9F8629-6B55-B242-BF24-8308AAED88DC}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
newest version for resubmission
</commit_message>
<xml_diff>
--- a/data/raw_data/degradation_curves_nsb.xlsx
+++ b/data/raw_data/degradation_curves_nsb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feraguilar/Library/CloudStorage/Box-Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DE147E-7C8B-C347-B985-C00607733FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8050C6B-EBD3-1448-8DDE-30B9744C9728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9780" yWindow="2560" windowWidth="27320" windowHeight="14860" xr2:uid="{92548F31-C31D-0241-8F30-7F9E6B95A567}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2821,277 +2820,222 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>161472</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22176E7F-319F-E742-9A5A-CF8D83823539}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2572102-AED0-4193-2D12-6174C2FA90BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>762001</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>69273</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>762001</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Connector 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F3FF7ED-3D49-ABFA-5AC9-2F0558E46737}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10033001" y="3602182"/>
-          <a:ext cx="0" cy="4260273"/>
+          <a:off x="3530105" y="878445"/>
+          <a:ext cx="10958945" cy="7803572"/>
+          <a:chOff x="3530105" y="878445"/>
+          <a:chExt cx="10958945" cy="7803572"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>221674</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>94673</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>221674</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>184727</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Connector 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA1ED85-5807-704D-9B01-9C6FDD2543EE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11155219" y="5082309"/>
-          <a:ext cx="0" cy="2791691"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466437</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>96981</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466437</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DDEB3D-0C1F-B440-8655-51DD0E015FB0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8906164" y="4253345"/>
-          <a:ext cx="0" cy="3609110"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>496455</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>108527</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>501074</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Connector 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9D7B8D-C1E1-F940-88F1-01BF8CE841BF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="12261273" y="5511800"/>
-          <a:ext cx="4619" cy="2350655"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>168563</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>87745</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>173181</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>196272</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Straight Connector 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C823A33A-0F98-0541-8FA8-DEBE2E539812}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7777018" y="3828472"/>
-          <a:ext cx="4618" cy="4057073"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Chart 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22176E7F-319F-E742-9A5A-CF8D83823539}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="3530105" y="878445"/>
+          <a:ext cx="10958945" cy="7803572"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="Straight Connector 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F3FF7ED-3D49-ABFA-5AC9-2F0558E46737}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10033001" y="3602182"/>
+            <a:ext cx="0" cy="4260273"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Straight Connector 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA1ED85-5807-704D-9B01-9C6FDD2543EE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11155219" y="5082309"/>
+            <a:ext cx="0" cy="2791691"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="9" name="Straight Connector 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DDEB3D-0C1F-B440-8655-51DD0E015FB0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8906164" y="4253345"/>
+            <a:ext cx="0" cy="3609110"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="15" name="Straight Connector 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9D7B8D-C1E1-F940-88F1-01BF8CE841BF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="12261273" y="5511800"/>
+            <a:ext cx="4619" cy="2350655"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="17" name="Straight Connector 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C823A33A-0F98-0541-8FA8-DEBE2E539812}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7777018" y="3828472"/>
+            <a:ext cx="4618" cy="4057073"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3478,7 +3422,7 @@
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>99% of</a:t>
+            <a:t>95% of</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1600" baseline="0">
@@ -3849,7 +3793,7 @@
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>